<commit_message>
modified:   Change_FullName_Account/file_fullname.xlsx 	modified:   Change_FullName_Account/ps_changefullname.ps1
</commit_message>
<xml_diff>
--- a/Change_FullName_Account/file_fullname.xlsx
+++ b/Change_FullName_Account/file_fullname.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06916B1-ECFE-433D-A5EB-A8B7E6518B3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A62320-F794-4015-8D1C-185DE75ACD61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,36 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>UserName</t>
   </si>
   <si>
-    <t>ComputerName</t>
+    <t>Display Name</t>
   </si>
   <si>
-    <t>sanglv1</t>
+    <t>sanglv</t>
   </si>
   <si>
-    <t>sanglv2</t>
-  </si>
-  <si>
-    <t>sanglv3</t>
-  </si>
-  <si>
-    <t>sanglv4</t>
-  </si>
-  <si>
-    <t>MT-151</t>
-  </si>
-  <si>
-    <t>MT-152</t>
-  </si>
-  <si>
-    <t>MT-153</t>
-  </si>
-  <si>
-    <t>MT-154</t>
+    <t>[IT] LE VAN SANG</t>
   </si>
 </sst>
 </file>
@@ -367,10 +349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -392,31 +374,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>